<commit_message>
plot and report paraphraser prototype
</commit_message>
<xml_diff>
--- a/notebooks/prototype/parapharser/openai_vs_mixtral.xlsx
+++ b/notebooks/prototype/parapharser/openai_vs_mixtral.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clo36\repo\askem\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clo36\repo\askem\notebooks\prototype\parapharser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37DC877F-94EB-480E-B3EF-B3820557E170}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DADC4A9-C28F-47E3-87B7-1A00505AEF45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="29208" windowHeight="25296" tabRatio="639" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5220" yWindow="6336" windowWidth="31224" windowHeight="16524" tabRatio="639" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="costar_v1_compare_llm" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="241">
   <si>
     <t>paraphrased</t>
   </si>
@@ -1017,6 +1017,15 @@
 To help understand how quickly COVID-19 was spreading, it is important to consider two key factors: the basic reproduction number (R0), which refers to the average number of people each infected person will pass the virus on to, and the variation in this number (Rvar), which reflects the range of transmission rates observed among different populations.
 In summary, the first reported case of COVID-19 in Egypt was identified in mid-February 2020, with more cases emerging over the following weeks. By March 14th, there were 110 confirmed cases. To fully grasp the spread of this disease, it's essential to consider factors such as initial immunity, the contagiousness of early vs. later infection stages, and the R0 and Rvar values.</t>
     </r>
+  </si>
+  <si>
+    <t>OAI (COSTAR_V1)</t>
+  </si>
+  <si>
+    <t>MIXTRAL (COSTAR_V1)</t>
+  </si>
+  <si>
+    <t>Correlations</t>
   </si>
 </sst>
 </file>
@@ -1518,17 +1527,17 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1902,16 +1911,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4" t="s">
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
@@ -3447,13 +3456,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J61"/>
+  <dimension ref="A1:J63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G3" sqref="G3"/>
+      <selection pane="bottomRight" activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3468,43 +3477,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C1" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
+      <c r="C1" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
       <c r="F1" s="2"/>
-      <c r="G1" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
+      <c r="G1" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="6"/>
-      <c r="B2" s="7" t="s">
+      <c r="A2" s="4"/>
+      <c r="B2" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="7" t="s">
+      <c r="F2" s="6"/>
+      <c r="G2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="6" t="s">
         <v>177</v>
       </c>
     </row>
@@ -5012,6 +5021,19 @@
       <c r="I61" s="3">
         <f>AVERAGE(I3:I59)</f>
         <v>0.87645267603690147</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G63" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="H63" s="3">
+        <f>CORREL(D3:D59,H3:H59)</f>
+        <v>0.5048655761324905</v>
+      </c>
+      <c r="I63" s="3">
+        <f>CORREL(E3:E59,I3:I59)</f>
+        <v>0.53599212879072122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>